<commit_message>
add notes to form update development form name/enketo url
</commit_message>
<xml_diff>
--- a/ona_forms/asistencias-pagos.xlsx
+++ b/ona_forms/asistencias-pagos.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="141">
   <si>
     <t>type</t>
   </si>
@@ -434,6 +434,15 @@
   </si>
   <si>
     <t>Monto</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>Notas</t>
+  </si>
+  <si>
+    <t>multiline</t>
   </si>
 </sst>
 </file>
@@ -903,10 +912,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K20"/>
+  <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1164,7 +1173,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:10">
       <c r="A17" t="s">
         <v>111</v>
       </c>
@@ -1175,7 +1184,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:10">
       <c r="A18" t="s">
         <v>99</v>
       </c>
@@ -1189,19 +1198,32 @@
         <v>117</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:10">
       <c r="A19" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:10">
       <c r="A20" t="s">
         <v>73</v>
       </c>
     </row>
+    <row r="21" spans="1:10">
+      <c r="A21" t="s">
+        <v>71</v>
+      </c>
+      <c r="B21" t="s">
+        <v>138</v>
+      </c>
+      <c r="C21" t="s">
+        <v>139</v>
+      </c>
+      <c r="J21" t="s">
+        <v>140</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
form updated for june pending specs
</commit_message>
<xml_diff>
--- a/ona_forms/asistencias-pagos.xlsx
+++ b/ona_forms/asistencias-pagos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="26520" windowHeight="14840" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
     <sheet name="choices" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="151">
   <si>
     <t>type</t>
   </si>
@@ -352,12 +352,6 @@
     <t>${kind} = 'OTRO'</t>
   </si>
   <si>
-    <t>Puede introducir número usando teclado en el siguiente paso</t>
-  </si>
-  <si>
-    <t>Aparece en blanco si leyó tarjeta en el paso anterior</t>
-  </si>
-  <si>
     <t>secondary_teacher</t>
   </si>
   <si>
@@ -367,15 +361,9 @@
     <t>Profesor</t>
   </si>
   <si>
-    <t>Este profesor colecta los cobros de la clase</t>
-  </si>
-  <si>
     <t>Otro profesor</t>
   </si>
   <si>
-    <t>Este proferos dicta la clase pero no colecta</t>
-  </si>
-  <si>
     <t>Alumno</t>
   </si>
   <si>
@@ -419,6 +407,39 @@
   </si>
   <si>
     <t>multiline</t>
+  </si>
+  <si>
+    <t>Seleccione la fecha a la que imputarán los registros</t>
+  </si>
+  <si>
+    <t>Seleccione el curso según disciplina, día y lugar.</t>
+  </si>
+  <si>
+    <t>Este profesor colecta y rinde los cobros de la clase. El presenta se registra automáticamente.</t>
+  </si>
+  <si>
+    <t>Este profesor dicta la clase pero no se quedó con cobros. El presente se registra automáticamente.</t>
+  </si>
+  <si>
+    <t>Escanear la tarjeta, sino puede introducir número usando teclado en el siguiente paso</t>
+  </si>
+  <si>
+    <t>Aparece en blanco si leyó tarjeta en el paso anterior. Puede consignar solo el código, sin los prefijos alfanuméricos.</t>
+  </si>
+  <si>
+    <t>Mail del alumno. Se debe registrar siempre. Aun con alumnos por clase suelta de ser posible.</t>
+  </si>
+  <si>
+    <t>En caso afirmativo se consignará luego el pago. En caso negativo se registrará solo el presente del alumno.</t>
+  </si>
+  <si>
+    <t>Plan que se está abonando.</t>
+  </si>
+  <si>
+    <t>Otro monto fuera de los planes</t>
+  </si>
+  <si>
+    <t>Texto libre para consignar excepciones y comentarios.</t>
   </si>
   <si>
     <t>Sol</t>
@@ -458,13 +479,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -472,7 +492,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <u/>
@@ -480,7 +499,6 @@
       <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <u/>
@@ -488,14 +506,18 @@
       <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -506,7 +528,14 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left/>
       <right/>
@@ -515,100 +544,38 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="43">
+  <cellStyleXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="43">
+  <cellStyles count="12">
+    <cellStyle name="Bold text" xfId="4"/>
+    <cellStyle name="Col header" xfId="8"/>
+    <cellStyle name="Date" xfId="9"/>
+    <cellStyle name="Date &amp; time" xfId="11"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Money" xfId="6"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Number" xfId="5"/>
+    <cellStyle name="Percentage" xfId="7"/>
+    <cellStyle name="Text" xfId="3"/>
+    <cellStyle name="Time" xfId="10"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -620,10 +587,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:srgbClr val="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -930,6 +897,11 @@
         </a:fontRef>
       </a:style>
     </a:lnDef>
+    <a:txDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+    </a:txDef>
   </a:objectDefaults>
   <a:extraClrSchemeLst/>
 </a:theme>
@@ -1012,7 +984,10 @@
         <v>77</v>
       </c>
       <c r="C4" t="s">
-        <v>113</v>
+        <v>111</v>
+      </c>
+      <c r="D4" t="s">
+        <v>129</v>
       </c>
       <c r="E4" t="s">
         <v>18</v>
@@ -1034,6 +1009,9 @@
       <c r="C5" t="s">
         <v>17</v>
       </c>
+      <c r="D5" t="s">
+        <v>130</v>
+      </c>
       <c r="E5" t="s">
         <v>18</v>
       </c>
@@ -1046,13 +1024,10 @@
         <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D6" t="s">
-        <v>115</v>
-      </c>
-      <c r="E6" t="s">
-        <v>18</v>
+        <v>131</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -1060,13 +1035,13 @@
         <v>90</v>
       </c>
       <c r="B7" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C7" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D7" t="s">
-        <v>117</v>
+        <v>132</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -1077,7 +1052,7 @@
         <v>60</v>
       </c>
       <c r="C8" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -1105,10 +1080,10 @@
         <v>62</v>
       </c>
       <c r="C10" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="D10" t="s">
-        <v>110</v>
+        <v>133</v>
       </c>
       <c r="H10" t="s">
         <v>88</v>
@@ -1122,10 +1097,10 @@
         <v>66</v>
       </c>
       <c r="C11" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D11" t="s">
-        <v>111</v>
+        <v>134</v>
       </c>
       <c r="H11" t="s">
         <v>88</v>
@@ -1139,7 +1114,13 @@
         <v>61</v>
       </c>
       <c r="C12" t="s">
-        <v>121</v>
+        <v>117</v>
+      </c>
+      <c r="D12" t="s">
+        <v>135</v>
+      </c>
+      <c r="E12" t="s">
+        <v>18</v>
       </c>
       <c r="H12" t="s">
         <v>89</v>
@@ -1150,10 +1131,10 @@
         <v>63</v>
       </c>
       <c r="B13" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C13" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="E13" t="s">
         <v>18</v>
@@ -1167,10 +1148,10 @@
         <v>63</v>
       </c>
       <c r="B14" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C14" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="H14" t="s">
         <v>89</v>
@@ -1184,7 +1165,10 @@
         <v>75</v>
       </c>
       <c r="C15" t="s">
-        <v>126</v>
+        <v>122</v>
+      </c>
+      <c r="D15" t="s">
+        <v>136</v>
       </c>
       <c r="I15" t="s">
         <v>69</v>
@@ -1198,7 +1182,7 @@
         <v>70</v>
       </c>
       <c r="C16" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="H16" t="s">
         <v>76</v>
@@ -1212,7 +1196,10 @@
         <v>74</v>
       </c>
       <c r="C17" t="s">
-        <v>128</v>
+        <v>124</v>
+      </c>
+      <c r="D17" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -1223,7 +1210,10 @@
         <v>73</v>
       </c>
       <c r="C18" t="s">
-        <v>129</v>
+        <v>125</v>
+      </c>
+      <c r="D18" t="s">
+        <v>138</v>
       </c>
       <c r="H18" t="s">
         <v>109</v>
@@ -1244,13 +1234,16 @@
         <v>63</v>
       </c>
       <c r="B21" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C21" t="s">
-        <v>131</v>
+        <v>127</v>
+      </c>
+      <c r="D21" t="s">
+        <v>139</v>
       </c>
       <c r="J21" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -1267,15 +1260,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView topLeftCell="B13" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="44.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1">
@@ -1296,10 +1289,13 @@
       <c r="A2" t="s">
         <v>15</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" s="2" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1307,10 +1303,13 @@
       <c r="A3" t="s">
         <v>15</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" s="2" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1318,10 +1317,13 @@
       <c r="A4" t="s">
         <v>15</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" s="2" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1329,10 +1331,13 @@
       <c r="A5" t="s">
         <v>15</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" s="2" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1340,10 +1345,13 @@
       <c r="A6" t="s">
         <v>15</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" s="2" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1351,10 +1359,13 @@
       <c r="A7" t="s">
         <v>15</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" s="2" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1362,32 +1373,46 @@
       <c r="A8" t="s">
         <v>15</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="2" t="s">
+      <c r="B9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>133</v>
-      </c>
       <c r="C9" s="2" t="s">
-        <v>133</v>
-      </c>
+        <v>140</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
         <v>16</v>
       </c>
       <c r="B11" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="D11" s="2" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1396,9 +1421,12 @@
         <v>16</v>
       </c>
       <c r="B12" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="D12" s="2" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1407,9 +1435,12 @@
         <v>16</v>
       </c>
       <c r="B13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="D13" s="2" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1418,9 +1449,12 @@
         <v>16</v>
       </c>
       <c r="B14" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="D14" s="2" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1429,9 +1463,12 @@
         <v>16</v>
       </c>
       <c r="B15" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="D15" s="2" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1440,295 +1477,385 @@
         <v>16</v>
       </c>
       <c r="B16" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="D16" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:4">
       <c r="A17" t="s">
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="D17" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:4">
       <c r="A18" t="s">
         <v>16</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>134</v>
+        <v>16</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
+        <v>141</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
       <c r="A19" t="s">
         <v>16</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>136</v>
+        <v>16</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
+        <v>143</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
       <c r="A20" t="s">
         <v>16</v>
       </c>
       <c r="B20" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="D20" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:4">
       <c r="A21" t="s">
         <v>16</v>
       </c>
       <c r="B21" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="D21" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:4">
       <c r="A22" t="s">
         <v>16</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>138</v>
+        <v>16</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
+        <v>145</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
       <c r="A23" t="s">
         <v>16</v>
       </c>
       <c r="B23" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="D23" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:4">
       <c r="A24" t="s">
         <v>16</v>
       </c>
       <c r="B24" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="D24" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:4">
       <c r="A25" t="s">
         <v>16</v>
       </c>
       <c r="B25" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C25" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="D25" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:4">
       <c r="A26" t="s">
         <v>16</v>
       </c>
       <c r="B26" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C26" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="D26" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:4">
       <c r="A27" t="s">
         <v>16</v>
       </c>
       <c r="B27" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C27" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="D27" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:4">
       <c r="A28" t="s">
         <v>16</v>
       </c>
       <c r="B28" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C28" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="D28" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:4">
       <c r="A29" t="s">
         <v>16</v>
       </c>
       <c r="B29" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C29" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="D29" s="2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
-      <c r="A30" t="s">
-        <v>16</v>
-      </c>
+    <row r="30" spans="1:4">
       <c r="B30" s="2" t="s">
-        <v>140</v>
+        <v>16</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3">
+        <v>147</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>16</v>
+        <v>68</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>142</v>
+        <v>16</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3">
-      <c r="A33" t="s">
+        <v>149</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" t="s">
         <v>68</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="B33" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C33" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C33" t="s">
+      <c r="D33" s="2" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:4">
       <c r="A34" t="s">
+        <v>78</v>
+      </c>
+      <c r="B34" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B34" t="s">
+      <c r="C34" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C34" t="s">
+      <c r="D34" s="2" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="35" spans="1:4">
+      <c r="A35" t="s">
+        <v>78</v>
+      </c>
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+    </row>
+    <row r="36" spans="1:4">
       <c r="A36" t="s">
         <v>78</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C36" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="C36" t="s">
+      <c r="D36" s="2" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
-      <c r="A37" t="s">
+    <row r="37" spans="1:4">
+      <c r="B37" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B37" t="s">
+      <c r="C37" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="C37" t="s">
+      <c r="D37" s="2" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
+    <row r="38" spans="1:4">
       <c r="A38" t="s">
+        <v>92</v>
+      </c>
+      <c r="B38" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B38" t="s">
+      <c r="C38" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="C38" t="s">
+      <c r="D38" s="2" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
+    <row r="39" spans="1:4">
+      <c r="A39" t="s">
+        <v>92</v>
+      </c>
+      <c r="B39" s="2"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="2"/>
+    </row>
+    <row r="40" spans="1:4">
       <c r="A40" t="s">
         <v>92</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C40" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="C40" t="s">
+      <c r="D40" s="2" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:4">
       <c r="A41" t="s">
         <v>92</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B41" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C41" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="C41" t="s">
+      <c r="D41" s="2" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="42" spans="1:3">
+    <row r="42" spans="1:4">
       <c r="A42" t="s">
         <v>92</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B42" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C42" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="C42" t="s">
+      <c r="D42" s="2" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="43" spans="1:3">
+    <row r="43" spans="1:4">
       <c r="A43" t="s">
         <v>92</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B43" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C43" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="C43" t="s">
+      <c r="D43" s="2" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="44" spans="1:3">
-      <c r="A44" t="s">
+    <row r="44" spans="1:4">
+      <c r="B44" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="B44" t="s">
+      <c r="C44" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="C44" t="s">
+      <c r="D44" s="2" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="45" spans="1:3">
-      <c r="A45" t="s">
+    <row r="45" spans="1:4">
+      <c r="B45" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="B45" t="s">
+      <c r="C45" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="C45" t="s">
+      <c r="D45" s="2" t="s">
         <v>108</v>
       </c>
     </row>

</xml_diff>

<commit_message>
bypass model validation again :-(
</commit_message>
<xml_diff>
--- a/ona_forms/asistencias-pagos.xlsx
+++ b/ona_forms/asistencias-pagos.xlsx
@@ -10,7 +10,7 @@
     <sheet name="survey" sheetId="1" r:id="rId1"/>
     <sheet name="choices" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="155">
   <si>
     <t>type</t>
   </si>
@@ -473,6 +473,18 @@
   </si>
   <si>
     <t>Tap - Principiantes - Viernes La huella</t>
+  </si>
+  <si>
+    <t>note</t>
+  </si>
+  <si>
+    <t>display</t>
+  </si>
+  <si>
+    <t>Recuerde cobrar los $15 por la tarjeta. Se los registra automáticamente.</t>
+  </si>
+  <si>
+    <t>${id_kind} = 'new_card'</t>
   </si>
 </sst>
 </file>
@@ -544,7 +556,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="12">
+  <cellStyleXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -557,19 +569,27 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="12">
+  <cellStyles count="16">
     <cellStyle name="Bold text" xfId="4"/>
     <cellStyle name="Col header" xfId="8"/>
     <cellStyle name="Date" xfId="9"/>
     <cellStyle name="Date &amp; time" xfId="11"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="15" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="12" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="14" builtinId="8" hidden="1"/>
     <cellStyle name="Money" xfId="6"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Number" xfId="5"/>
@@ -909,10 +929,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K21"/>
+  <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1029,6 +1049,9 @@
       <c r="D6" t="s">
         <v>131</v>
       </c>
+      <c r="E6" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="7" spans="1:11">
       <c r="A7" t="s">
@@ -1074,33 +1097,30 @@
     </row>
     <row r="10" spans="1:11">
       <c r="A10" t="s">
-        <v>64</v>
+        <v>151</v>
       </c>
       <c r="B10" t="s">
-        <v>62</v>
-      </c>
-      <c r="C10" t="s">
-        <v>115</v>
+        <v>152</v>
       </c>
       <c r="D10" t="s">
-        <v>133</v>
-      </c>
-      <c r="H10" t="s">
-        <v>88</v>
+        <v>153</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="11" spans="1:11">
       <c r="A11" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B11" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D11" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H11" t="s">
         <v>88</v>
@@ -1111,19 +1131,16 @@
         <v>63</v>
       </c>
       <c r="B12" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="C12" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D12" t="s">
-        <v>135</v>
-      </c>
-      <c r="E12" t="s">
-        <v>18</v>
+        <v>134</v>
       </c>
       <c r="H12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -1131,10 +1148,13 @@
         <v>63</v>
       </c>
       <c r="B13" t="s">
-        <v>119</v>
+        <v>61</v>
       </c>
       <c r="C13" t="s">
-        <v>118</v>
+        <v>117</v>
+      </c>
+      <c r="D13" t="s">
+        <v>135</v>
       </c>
       <c r="E13" t="s">
         <v>18</v>
@@ -1148,10 +1168,13 @@
         <v>63</v>
       </c>
       <c r="B14" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C14" t="s">
-        <v>121</v>
+        <v>118</v>
+      </c>
+      <c r="E14" t="s">
+        <v>18</v>
       </c>
       <c r="H14" t="s">
         <v>89</v>
@@ -1159,95 +1182,110 @@
     </row>
     <row r="15" spans="1:11">
       <c r="A15" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B15" t="s">
-        <v>75</v>
+        <v>120</v>
       </c>
       <c r="C15" t="s">
-        <v>122</v>
-      </c>
-      <c r="D15" t="s">
-        <v>136</v>
-      </c>
-      <c r="I15" t="s">
-        <v>69</v>
+        <v>121</v>
+      </c>
+      <c r="H15" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="16" spans="1:11">
       <c r="A16" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B16" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="C16" t="s">
-        <v>123</v>
-      </c>
-      <c r="H16" t="s">
-        <v>76</v>
+        <v>122</v>
+      </c>
+      <c r="D16" t="s">
+        <v>136</v>
+      </c>
+      <c r="I16" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="17" spans="1:10">
       <c r="A17" t="s">
-        <v>103</v>
+        <v>71</v>
       </c>
       <c r="B17" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C17" t="s">
-        <v>124</v>
-      </c>
-      <c r="D17" t="s">
-        <v>137</v>
+        <v>123</v>
+      </c>
+      <c r="H17" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="18" spans="1:10">
       <c r="A18" t="s">
-        <v>91</v>
+        <v>103</v>
       </c>
       <c r="B18" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C18" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D18" t="s">
-        <v>138</v>
-      </c>
-      <c r="H18" t="s">
-        <v>109</v>
+        <v>137</v>
       </c>
     </row>
     <row r="19" spans="1:10">
       <c r="A19" t="s">
-        <v>72</v>
+        <v>91</v>
+      </c>
+      <c r="B19" t="s">
+        <v>73</v>
+      </c>
+      <c r="C19" t="s">
+        <v>125</v>
+      </c>
+      <c r="D19" t="s">
+        <v>138</v>
+      </c>
+      <c r="H19" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="A22" t="s">
         <v>63</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B22" t="s">
         <v>126</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C22" t="s">
         <v>127</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D22" t="s">
         <v>139</v>
       </c>
-      <c r="J21" t="s">
+      <c r="J22" t="s">
         <v>128</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1260,8 +1298,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D45"/>
   <sheetViews>
-    <sheetView topLeftCell="B13" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:D45"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1286,578 +1324,508 @@
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>20</v>
-      </c>
+      <c r="D2" s="2"/>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" t="s">
+      <c r="A3" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>21</v>
-      </c>
+      <c r="D3" s="2"/>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" t="s">
+      <c r="A4" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>22</v>
-      </c>
+      <c r="D4" s="2"/>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" t="s">
+      <c r="A5" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>23</v>
-      </c>
+      <c r="D5" s="2"/>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" t="s">
+      <c r="A6" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>24</v>
-      </c>
+      <c r="D6" s="2"/>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" t="s">
+      <c r="A7" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>25</v>
-      </c>
+      <c r="D7" s="2"/>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" t="s">
+      <c r="A8" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>26</v>
-      </c>
+      <c r="D8" s="2"/>
     </row>
     <row r="9" spans="1:4">
+      <c r="A9" s="2" t="s">
+        <v>15</v>
+      </c>
       <c r="B9" s="2" t="s">
-        <v>15</v>
+        <v>140</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>140</v>
-      </c>
+      <c r="D9" s="2"/>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" t="s">
-        <v>16</v>
-      </c>
+      <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" t="s">
+      <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>16</v>
+        <v>57</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="D11" s="2" t="s">
         <v>58</v>
       </c>
+      <c r="D11" s="2"/>
     </row>
     <row r="12" spans="1:4">
-      <c r="A12" t="s">
+      <c r="A12" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D12" s="2" t="s">
         <v>28</v>
       </c>
+      <c r="D12" s="2"/>
     </row>
     <row r="13" spans="1:4">
-      <c r="A13" t="s">
+      <c r="A13" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D13" s="2" t="s">
         <v>30</v>
       </c>
+      <c r="D13" s="2"/>
     </row>
     <row r="14" spans="1:4">
-      <c r="A14" t="s">
+      <c r="A14" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D14" s="2" t="s">
         <v>32</v>
       </c>
+      <c r="D14" s="2"/>
     </row>
     <row r="15" spans="1:4">
-      <c r="A15" t="s">
+      <c r="A15" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D15" s="2" t="s">
         <v>34</v>
       </c>
+      <c r="D15" s="2"/>
     </row>
     <row r="16" spans="1:4">
-      <c r="A16" t="s">
+      <c r="A16" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D16" s="2" t="s">
         <v>36</v>
       </c>
+      <c r="D16" s="2"/>
     </row>
     <row r="17" spans="1:4">
-      <c r="A17" t="s">
+      <c r="A17" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>16</v>
+        <v>37</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D17" s="2" t="s">
         <v>38</v>
       </c>
+      <c r="D17" s="2"/>
     </row>
     <row r="18" spans="1:4">
-      <c r="A18" t="s">
+      <c r="A18" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>16</v>
+        <v>141</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="D18" s="2" t="s">
         <v>142</v>
       </c>
+      <c r="D18" s="2"/>
     </row>
     <row r="19" spans="1:4">
-      <c r="A19" t="s">
+      <c r="A19" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>16</v>
+        <v>143</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="D19" s="2" t="s">
         <v>144</v>
       </c>
+      <c r="D19" s="2"/>
     </row>
     <row r="20" spans="1:4">
-      <c r="A20" t="s">
+      <c r="A20" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>16</v>
+        <v>39</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D20" s="2" t="s">
         <v>40</v>
       </c>
+      <c r="D20" s="2"/>
     </row>
     <row r="21" spans="1:4">
-      <c r="A21" t="s">
+      <c r="A21" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D21" s="2" t="s">
         <v>42</v>
       </c>
+      <c r="D21" s="2"/>
     </row>
     <row r="22" spans="1:4">
-      <c r="A22" t="s">
+      <c r="A22" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>16</v>
+        <v>145</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="D22" s="2" t="s">
         <v>146</v>
       </c>
+      <c r="D22" s="2"/>
     </row>
     <row r="23" spans="1:4">
-      <c r="A23" t="s">
+      <c r="A23" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D23" s="2" t="s">
         <v>44</v>
       </c>
+      <c r="D23" s="2"/>
     </row>
     <row r="24" spans="1:4">
-      <c r="A24" t="s">
+      <c r="A24" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D24" s="2" t="s">
         <v>46</v>
       </c>
+      <c r="D24" s="2"/>
     </row>
     <row r="25" spans="1:4">
-      <c r="A25" t="s">
+      <c r="A25" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>16</v>
+        <v>47</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D25" s="2" t="s">
         <v>48</v>
       </c>
+      <c r="D25" s="2"/>
     </row>
     <row r="26" spans="1:4">
-      <c r="A26" t="s">
+      <c r="A26" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>16</v>
+        <v>49</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="D26" s="2" t="s">
         <v>50</v>
       </c>
+      <c r="D26" s="2"/>
     </row>
     <row r="27" spans="1:4">
-      <c r="A27" t="s">
+      <c r="A27" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>16</v>
+        <v>51</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D27" s="2" t="s">
         <v>52</v>
       </c>
+      <c r="D27" s="2"/>
     </row>
     <row r="28" spans="1:4">
-      <c r="A28" t="s">
+      <c r="A28" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>16</v>
+        <v>53</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D28" s="2" t="s">
         <v>54</v>
       </c>
+      <c r="D28" s="2"/>
     </row>
     <row r="29" spans="1:4">
-      <c r="A29" t="s">
+      <c r="A29" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>16</v>
+        <v>55</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="D29" s="2" t="s">
         <v>56</v>
       </c>
+      <c r="D29" s="2"/>
     </row>
     <row r="30" spans="1:4">
+      <c r="A30" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="B30" s="2" t="s">
-        <v>16</v>
+        <v>147</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="D30" s="2" t="s">
         <v>148</v>
       </c>
+      <c r="D30" s="2"/>
     </row>
     <row r="31" spans="1:4">
-      <c r="A31" t="s">
-        <v>68</v>
+      <c r="A31" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>16</v>
+        <v>149</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="D31" s="2" t="s">
         <v>150</v>
       </c>
+      <c r="D31" s="2"/>
     </row>
     <row r="32" spans="1:4">
-      <c r="A32" t="s">
-        <v>68</v>
-      </c>
+      <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
     </row>
     <row r="33" spans="1:4">
+      <c r="A33" s="2" t="s">
+        <v>68</v>
+      </c>
       <c r="B33" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D33" s="2"/>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C33" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4">
-      <c r="A34" t="s">
-        <v>78</v>
-      </c>
       <c r="B34" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="D34" s="2" t="s">
         <v>106</v>
       </c>
+      <c r="D34" s="2"/>
     </row>
     <row r="35" spans="1:4">
-      <c r="A35" t="s">
-        <v>78</v>
-      </c>
+      <c r="A35" s="2"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
     </row>
     <row r="36" spans="1:4">
-      <c r="A36" t="s">
+      <c r="A36" s="2" t="s">
         <v>78</v>
       </c>
       <c r="B36" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D36" s="2"/>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="C36" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4">
       <c r="B37" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D37" s="2"/>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="C37" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4">
-      <c r="A38" t="s">
-        <v>92</v>
-      </c>
       <c r="B38" s="2" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="D38" s="2" t="s">
         <v>84</v>
       </c>
+      <c r="D38" s="2"/>
     </row>
     <row r="39" spans="1:4">
-      <c r="A39" t="s">
-        <v>92</v>
-      </c>
+      <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
     </row>
     <row r="40" spans="1:4">
-      <c r="A40" t="s">
+      <c r="A40" s="2" t="s">
         <v>92</v>
       </c>
       <c r="B40" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D40" s="2"/>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="C40" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4">
-      <c r="A41" t="s">
+      <c r="B41" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D41" s="2"/>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="B42" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D42" s="2"/>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="C41" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4">
-      <c r="A42" t="s">
+      <c r="B43" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D43" s="2"/>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="B44" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D44" s="2"/>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="C42" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4">
-      <c r="A43" t="s">
-        <v>92</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4">
-      <c r="B44" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4">
       <c r="B45" s="2" t="s">
-        <v>92</v>
+        <v>107</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="D45" s="2" t="s">
         <v>108</v>
       </c>
+      <c r="D45" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
add missing class LH_INT1_SAB
</commit_message>
<xml_diff>
--- a/ona_forms/asistencias-pagos.xlsx
+++ b/ona_forms/asistencias-pagos.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="26520" windowHeight="14840" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="26520" windowHeight="14840" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="157">
   <si>
     <t>type</t>
   </si>
@@ -485,6 +485,12 @@
   </si>
   <si>
     <t>${id_kind} = 'new_card'</t>
+  </si>
+  <si>
+    <t>LH_INT1_SAB</t>
+  </si>
+  <si>
+    <t>Lindy Hop - Intermedios 1 - Sábados Sc</t>
   </si>
 </sst>
 </file>
@@ -556,7 +562,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="16">
+  <cellStyleXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -573,13 +579,15 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="16">
+  <cellStyles count="18">
     <cellStyle name="Bold text" xfId="4"/>
     <cellStyle name="Col header" xfId="8"/>
     <cellStyle name="Date" xfId="9"/>
@@ -587,9 +595,11 @@
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="15" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="17" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="12" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="14" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="16" builtinId="8" hidden="1"/>
     <cellStyle name="Money" xfId="6"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Number" xfId="5"/>
@@ -931,7 +941,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
@@ -1285,7 +1295,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1296,10 +1305,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D45"/>
+  <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1526,10 +1535,10 @@
         <v>16</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>143</v>
+        <v>155</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>144</v>
+        <v>156</v>
       </c>
       <c r="D19" s="2"/>
     </row>
@@ -1538,10 +1547,10 @@
         <v>16</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>39</v>
+        <v>143</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>40</v>
+        <v>144</v>
       </c>
       <c r="D20" s="2"/>
     </row>
@@ -1550,10 +1559,10 @@
         <v>16</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D21" s="2"/>
     </row>
@@ -1562,10 +1571,10 @@
         <v>16</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>145</v>
+        <v>41</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>146</v>
+        <v>42</v>
       </c>
       <c r="D22" s="2"/>
     </row>
@@ -1574,10 +1583,10 @@
         <v>16</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>43</v>
+        <v>145</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>44</v>
+        <v>146</v>
       </c>
       <c r="D23" s="2"/>
     </row>
@@ -1586,10 +1595,10 @@
         <v>16</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D24" s="2"/>
     </row>
@@ -1598,10 +1607,10 @@
         <v>16</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D25" s="2"/>
     </row>
@@ -1610,10 +1619,10 @@
         <v>16</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D26" s="2"/>
     </row>
@@ -1622,10 +1631,10 @@
         <v>16</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D27" s="2"/>
     </row>
@@ -1634,10 +1643,10 @@
         <v>16</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D28" s="2"/>
     </row>
@@ -1646,10 +1655,10 @@
         <v>16</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D29" s="2"/>
     </row>
@@ -1658,10 +1667,10 @@
         <v>16</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>147</v>
+        <v>55</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>148</v>
+        <v>56</v>
       </c>
       <c r="D30" s="2"/>
     </row>
@@ -1670,29 +1679,29 @@
         <v>16</v>
       </c>
       <c r="B31" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="D31" s="2"/>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B32" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="C32" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="D31" s="2"/>
-    </row>
-    <row r="32" spans="1:4">
-      <c r="A32" s="2"/>
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
       <c r="D32" s="2"/>
     </row>
     <row r="33" spans="1:4">
-      <c r="A33" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>105</v>
-      </c>
+      <c r="A33" s="2"/>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
       <c r="D33" s="2"/>
     </row>
     <row r="34" spans="1:4">
@@ -1700,29 +1709,29 @@
         <v>68</v>
       </c>
       <c r="B34" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D34" s="2"/>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B35" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="C35" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="D34" s="2"/>
-    </row>
-    <row r="35" spans="1:4">
-      <c r="A35" s="2"/>
-      <c r="B35" s="2"/>
-      <c r="C35" s="2"/>
       <c r="D35" s="2"/>
     </row>
     <row r="36" spans="1:4">
-      <c r="A36" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>82</v>
-      </c>
+      <c r="A36" s="2"/>
+      <c r="B36" s="2"/>
+      <c r="C36" s="2"/>
       <c r="D36" s="2"/>
     </row>
     <row r="37" spans="1:4">
@@ -1730,10 +1739,10 @@
         <v>78</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D37" s="2"/>
     </row>
@@ -1742,29 +1751,29 @@
         <v>78</v>
       </c>
       <c r="B38" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D38" s="2"/>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B39" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="C39" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="D38" s="2"/>
-    </row>
-    <row r="39" spans="1:4">
-      <c r="A39" s="2"/>
-      <c r="B39" s="2"/>
-      <c r="C39" s="2"/>
       <c r="D39" s="2"/>
     </row>
     <row r="40" spans="1:4">
-      <c r="A40" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>96</v>
-      </c>
+      <c r="A40" s="2"/>
+      <c r="B40" s="2"/>
+      <c r="C40" s="2"/>
       <c r="D40" s="2"/>
     </row>
     <row r="41" spans="1:4">
@@ -1772,10 +1781,10 @@
         <v>92</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D41" s="2"/>
     </row>
@@ -1784,10 +1793,10 @@
         <v>92</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D42" s="2"/>
     </row>
@@ -1796,10 +1805,10 @@
         <v>92</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D43" s="2"/>
     </row>
@@ -1808,10 +1817,10 @@
         <v>92</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D44" s="2"/>
     </row>
@@ -1820,15 +1829,28 @@
         <v>92</v>
       </c>
       <c r="B45" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D45" s="2"/>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B46" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="C45" s="2" t="s">
+      <c r="C46" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="D45" s="2"/>
+      <c r="D46" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
soruce courses by date. update ona form fixes #21
</commit_message>
<xml_diff>
--- a/ona_forms/asistencias-pagos.xlsx
+++ b/ona_forms/asistencias-pagos.xlsx
@@ -1308,7 +1308,7 @@
   <dimension ref="A1:D46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1439,10 +1439,10 @@
         <v>16</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>57</v>
+        <v>29</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>58</v>
+        <v>30</v>
       </c>
       <c r="D11" s="2"/>
     </row>
@@ -1451,10 +1451,10 @@
         <v>16</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="D12" s="2"/>
     </row>
@@ -1463,10 +1463,10 @@
         <v>16</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="D13" s="2"/>
     </row>
@@ -1475,10 +1475,10 @@
         <v>16</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="D14" s="2"/>
     </row>
@@ -1487,10 +1487,10 @@
         <v>16</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D15" s="2"/>
     </row>
@@ -1499,10 +1499,10 @@
         <v>16</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="D16" s="2"/>
     </row>
@@ -1511,10 +1511,10 @@
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>37</v>
+        <v>55</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
       <c r="D17" s="2"/>
     </row>
@@ -1523,10 +1523,10 @@
         <v>16</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>141</v>
+        <v>57</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>142</v>
+        <v>58</v>
       </c>
       <c r="D18" s="2"/>
     </row>
@@ -1535,10 +1535,10 @@
         <v>16</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>155</v>
+        <v>27</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>156</v>
+        <v>28</v>
       </c>
       <c r="D19" s="2"/>
     </row>
@@ -1547,10 +1547,10 @@
         <v>16</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>143</v>
+        <v>37</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>144</v>
+        <v>38</v>
       </c>
       <c r="D20" s="2"/>
     </row>
@@ -1559,10 +1559,10 @@
         <v>16</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="D21" s="2"/>
     </row>
@@ -1571,10 +1571,10 @@
         <v>16</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="D22" s="2"/>
     </row>
@@ -1583,10 +1583,10 @@
         <v>16</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>145</v>
+        <v>39</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>146</v>
+        <v>40</v>
       </c>
       <c r="D23" s="2"/>
     </row>
@@ -1607,10 +1607,10 @@
         <v>16</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>45</v>
+        <v>141</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>46</v>
+        <v>142</v>
       </c>
       <c r="D25" s="2"/>
     </row>
@@ -1619,10 +1619,10 @@
         <v>16</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>47</v>
+        <v>143</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>48</v>
+        <v>144</v>
       </c>
       <c r="D26" s="2"/>
     </row>
@@ -1631,10 +1631,10 @@
         <v>16</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="D27" s="2"/>
     </row>
@@ -1643,10 +1643,10 @@
         <v>16</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>51</v>
+        <v>147</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>52</v>
+        <v>148</v>
       </c>
       <c r="D28" s="2"/>
     </row>
@@ -1655,10 +1655,10 @@
         <v>16</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>53</v>
+        <v>149</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>54</v>
+        <v>150</v>
       </c>
       <c r="D29" s="2"/>
     </row>
@@ -1667,10 +1667,10 @@
         <v>16</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>55</v>
+        <v>155</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>56</v>
+        <v>156</v>
       </c>
       <c r="D30" s="2"/>
     </row>
@@ -1679,10 +1679,10 @@
         <v>16</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D31" s="2"/>
     </row>
@@ -1691,10 +1691,10 @@
         <v>16</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>149</v>
+        <v>51</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>150</v>
+        <v>52</v>
       </c>
       <c r="D32" s="2"/>
     </row>
@@ -1850,7 +1850,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
fixes #34 payment_plan 3 classes/week at $500
</commit_message>
<xml_diff>
--- a/ona_forms/asistencias-pagos.xlsx
+++ b/ona_forms/asistencias-pagos.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="159">
   <si>
     <t>type</t>
   </si>
@@ -491,6 +491,12 @@
   </si>
   <si>
     <t>Lindy Hop - Principiantes - Martes La Fragua</t>
+  </si>
+  <si>
+    <t>3_X_SEMANA</t>
+  </si>
+  <si>
+    <t>Mensual 3 x Semana $500</t>
   </si>
 </sst>
 </file>
@@ -562,7 +568,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="18">
+  <cellStyleXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -581,13 +587,15 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="18">
+  <cellStyles count="20">
     <cellStyle name="Bold text" xfId="4"/>
     <cellStyle name="Col header" xfId="8"/>
     <cellStyle name="Date" xfId="9"/>
@@ -596,10 +604,12 @@
     <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="15" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="17" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="19" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="12" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="14" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="16" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="18" builtinId="8" hidden="1"/>
     <cellStyle name="Money" xfId="6"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Number" xfId="5"/>
@@ -1305,10 +1315,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D46"/>
+  <dimension ref="A1:D47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1793,10 +1803,10 @@
         <v>90</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>91</v>
+        <v>157</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>95</v>
+        <v>158</v>
       </c>
       <c r="D42" s="2"/>
     </row>
@@ -1805,10 +1815,10 @@
         <v>90</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D43" s="2"/>
     </row>
@@ -1817,10 +1827,10 @@
         <v>90</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D44" s="2"/>
     </row>
@@ -1829,10 +1839,10 @@
         <v>90</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D45" s="2"/>
     </row>
@@ -1841,15 +1851,28 @@
         <v>90</v>
       </c>
       <c r="B46" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D46" s="2"/>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B47" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="C46" s="2" t="s">
+      <c r="C47" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="D46" s="2"/>
+      <c r="D47" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
#4 new payment plans fees
</commit_message>
<xml_diff>
--- a/ona_forms/asistencias-pagos.xlsx
+++ b/ona_forms/asistencias-pagos.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="161">
   <si>
     <t>type</t>
   </si>
@@ -307,9 +307,6 @@
     <t>3 Meses 1 x Semana $550</t>
   </si>
   <si>
-    <t>Mensual 2 x Semana $350</t>
-  </si>
-  <si>
     <t>1_X_SEMANA_5</t>
   </si>
   <si>
@@ -497,6 +494,15 @@
   </si>
   <si>
     <t>Mensual 3 x Semana $500</t>
+  </si>
+  <si>
+    <t>Mensual 2 x Semana $400</t>
+  </si>
+  <si>
+    <t>1_X_SEMANA_3</t>
+  </si>
+  <si>
+    <t>Mensual 1 x Semana (3 c) $180</t>
   </si>
 </sst>
 </file>
@@ -568,7 +574,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
+  <cellStyleXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -589,13 +595,15 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="20">
+  <cellStyles count="22">
     <cellStyle name="Bold text" xfId="4"/>
     <cellStyle name="Col header" xfId="8"/>
     <cellStyle name="Date" xfId="9"/>
@@ -605,11 +613,13 @@
     <cellStyle name="Followed Hyperlink" xfId="15" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="17" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="19" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="21" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="12" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="14" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="16" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="18" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="20" builtinId="8" hidden="1"/>
     <cellStyle name="Money" xfId="6"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Number" xfId="5"/>
@@ -1024,10 +1034,10 @@
         <v>75</v>
       </c>
       <c r="C4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E4" t="s">
         <v>18</v>
@@ -1036,7 +1046,7 @@
         <v>13</v>
       </c>
       <c r="J4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -1050,7 +1060,7 @@
         <v>17</v>
       </c>
       <c r="D5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E5" t="s">
         <v>18</v>
@@ -1064,10 +1074,10 @@
         <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E6" t="s">
         <v>18</v>
@@ -1078,13 +1088,13 @@
         <v>88</v>
       </c>
       <c r="B7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -1095,7 +1105,7 @@
         <v>58</v>
       </c>
       <c r="C8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -1117,16 +1127,16 @@
     </row>
     <row r="10" spans="1:11">
       <c r="A10" t="s">
+        <v>148</v>
+      </c>
+      <c r="B10" t="s">
         <v>149</v>
       </c>
-      <c r="B10" t="s">
+      <c r="D10" t="s">
         <v>150</v>
       </c>
-      <c r="D10" t="s">
+      <c r="H10" s="2" t="s">
         <v>151</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -1137,10 +1147,10 @@
         <v>60</v>
       </c>
       <c r="C11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D11" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H11" t="s">
         <v>86</v>
@@ -1154,10 +1164,10 @@
         <v>64</v>
       </c>
       <c r="C12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D12" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H12" t="s">
         <v>86</v>
@@ -1171,10 +1181,10 @@
         <v>59</v>
       </c>
       <c r="C13" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D13" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E13" t="s">
         <v>18</v>
@@ -1188,10 +1198,10 @@
         <v>61</v>
       </c>
       <c r="B14" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C14" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E14" t="s">
         <v>18</v>
@@ -1205,10 +1215,10 @@
         <v>61</v>
       </c>
       <c r="B15" t="s">
+        <v>117</v>
+      </c>
+      <c r="C15" t="s">
         <v>118</v>
-      </c>
-      <c r="C15" t="s">
-        <v>119</v>
       </c>
       <c r="H15" t="s">
         <v>87</v>
@@ -1222,10 +1232,10 @@
         <v>73</v>
       </c>
       <c r="C16" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D16" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I16" t="s">
         <v>67</v>
@@ -1239,7 +1249,7 @@
         <v>68</v>
       </c>
       <c r="C17" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H17" t="s">
         <v>74</v>
@@ -1247,16 +1257,16 @@
     </row>
     <row r="18" spans="1:10">
       <c r="A18" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B18" t="s">
         <v>72</v>
       </c>
       <c r="C18" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D18" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -1267,13 +1277,13 @@
         <v>71</v>
       </c>
       <c r="C19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D19" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H19" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -1291,16 +1301,16 @@
         <v>61</v>
       </c>
       <c r="B22" t="s">
+        <v>123</v>
+      </c>
+      <c r="C22" t="s">
         <v>124</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
+        <v>136</v>
+      </c>
+      <c r="J22" t="s">
         <v>125</v>
-      </c>
-      <c r="D22" t="s">
-        <v>137</v>
-      </c>
-      <c r="J22" t="s">
-        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -1315,10 +1325,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D47"/>
+  <dimension ref="A1:D48"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1431,10 +1441,10 @@
         <v>15</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D9" s="2"/>
     </row>
@@ -1500,7 +1510,7 @@
         <v>35</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D15" s="2"/>
     </row>
@@ -1512,7 +1522,7 @@
         <v>46</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D16" s="2"/>
     </row>
@@ -1617,10 +1627,10 @@
         <v>16</v>
       </c>
       <c r="B25" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="C25" s="2" t="s">
         <v>139</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>140</v>
       </c>
       <c r="D25" s="2"/>
     </row>
@@ -1629,10 +1639,10 @@
         <v>16</v>
       </c>
       <c r="B26" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C26" s="2" t="s">
         <v>141</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>142</v>
       </c>
       <c r="D26" s="2"/>
     </row>
@@ -1653,10 +1663,10 @@
         <v>16</v>
       </c>
       <c r="B28" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="C28" s="2" t="s">
         <v>145</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>146</v>
       </c>
       <c r="D28" s="2"/>
     </row>
@@ -1665,10 +1675,10 @@
         <v>16</v>
       </c>
       <c r="B29" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="C29" s="2" t="s">
         <v>147</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>148</v>
       </c>
       <c r="D29" s="2"/>
     </row>
@@ -1677,10 +1687,10 @@
         <v>16</v>
       </c>
       <c r="B30" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="C30" s="2" t="s">
         <v>153</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>154</v>
       </c>
       <c r="D30" s="2"/>
     </row>
@@ -1689,10 +1699,10 @@
         <v>16</v>
       </c>
       <c r="B31" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="C31" s="2" t="s">
         <v>143</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>144</v>
       </c>
       <c r="D31" s="2"/>
     </row>
@@ -1722,7 +1732,7 @@
         <v>18</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D34" s="2"/>
     </row>
@@ -1734,7 +1744,7 @@
         <v>67</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D35" s="2"/>
     </row>
@@ -1803,10 +1813,10 @@
         <v>90</v>
       </c>
       <c r="B42" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="C42" s="2" t="s">
         <v>157</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>158</v>
       </c>
       <c r="D42" s="2"/>
     </row>
@@ -1818,7 +1828,7 @@
         <v>91</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>95</v>
+        <v>158</v>
       </c>
       <c r="D43" s="2"/>
     </row>
@@ -1827,10 +1837,10 @@
         <v>90</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>97</v>
+        <v>159</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>98</v>
+        <v>160</v>
       </c>
       <c r="D44" s="2"/>
     </row>
@@ -1842,7 +1852,7 @@
         <v>96</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D45" s="2"/>
     </row>
@@ -1851,10 +1861,10 @@
         <v>90</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D46" s="2"/>
     </row>
@@ -1863,12 +1873,24 @@
         <v>90</v>
       </c>
       <c r="B47" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D47" s="2"/>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C48" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="C47" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="D47" s="2"/>
+      <c r="D48" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
limbo classes fixes #36. wordpress integration
</commit_message>
<xml_diff>
--- a/ona_forms/asistencias-pagos.xlsx
+++ b/ona_forms/asistencias-pagos.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="167">
   <si>
     <t>type</t>
   </si>
@@ -503,6 +503,24 @@
   </si>
   <si>
     <t>Mensual 1 x Semana (3 c) $180</t>
+  </si>
+  <si>
+    <t>LIMBO_2</t>
+  </si>
+  <si>
+    <t>LIMBO_1</t>
+  </si>
+  <si>
+    <t>LIMBO_3</t>
+  </si>
+  <si>
+    <t>Limbo 3 - Intermedios 2 - Viernes Vera</t>
+  </si>
+  <si>
+    <t>Limbo 2 - Intermedios 1 - Miércoles Sendas</t>
+  </si>
+  <si>
+    <t>Limbo 1 - Principiantes - Miércoles Sendas</t>
   </si>
 </sst>
 </file>
@@ -574,7 +592,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="22">
+  <cellStyleXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -597,13 +615,15 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="22">
+  <cellStyles count="24">
     <cellStyle name="Bold text" xfId="4"/>
     <cellStyle name="Col header" xfId="8"/>
     <cellStyle name="Date" xfId="9"/>
@@ -614,12 +634,14 @@
     <cellStyle name="Followed Hyperlink" xfId="17" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="19" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="21" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="23" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="12" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="14" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="16" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="18" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="20" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="22" builtinId="8" hidden="1"/>
     <cellStyle name="Money" xfId="6"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Number" xfId="5"/>
@@ -1325,10 +1347,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D48"/>
+  <dimension ref="A1:D52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1458,11 +1480,11 @@
       <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>30</v>
+      <c r="B11" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" t="s">
+        <v>41</v>
       </c>
       <c r="D11" s="2"/>
     </row>
@@ -1470,11 +1492,11 @@
       <c r="A12" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>34</v>
+      <c r="B12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12" t="s">
+        <v>45</v>
       </c>
       <c r="D12" s="2"/>
     </row>
@@ -1482,11 +1504,11 @@
       <c r="A13" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>41</v>
+      <c r="B13" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" t="s">
+        <v>30</v>
       </c>
       <c r="D13" s="2"/>
     </row>
@@ -1494,11 +1516,11 @@
       <c r="A14" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>45</v>
+      <c r="B14" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" t="s">
+        <v>34</v>
       </c>
       <c r="D14" s="2"/>
     </row>
@@ -1506,11 +1528,11 @@
       <c r="A15" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>154</v>
+      <c r="B15" t="s">
+        <v>53</v>
+      </c>
+      <c r="C15" t="s">
+        <v>54</v>
       </c>
       <c r="D15" s="2"/>
     </row>
@@ -1518,11 +1540,11 @@
       <c r="A16" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>155</v>
+      <c r="B16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" t="s">
+        <v>154</v>
       </c>
       <c r="D16" s="2"/>
     </row>
@@ -1530,11 +1552,11 @@
       <c r="A17" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>54</v>
+      <c r="B17" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" t="s">
+        <v>155</v>
       </c>
       <c r="D17" s="2"/>
     </row>
@@ -1542,11 +1564,11 @@
       <c r="A18" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>56</v>
+      <c r="B18" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" t="s">
+        <v>37</v>
       </c>
       <c r="D18" s="2"/>
     </row>
@@ -1554,11 +1576,11 @@
       <c r="A19" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>28</v>
+      <c r="B19" t="s">
+        <v>47</v>
+      </c>
+      <c r="C19" t="s">
+        <v>48</v>
       </c>
       <c r="D19" s="2"/>
     </row>
@@ -1566,11 +1588,11 @@
       <c r="A20" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>37</v>
+      <c r="B20" t="s">
+        <v>161</v>
+      </c>
+      <c r="C20" t="s">
+        <v>165</v>
       </c>
       <c r="D20" s="2"/>
     </row>
@@ -1578,11 +1600,11 @@
       <c r="A21" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>48</v>
+      <c r="B21" t="s">
+        <v>55</v>
+      </c>
+      <c r="C21" t="s">
+        <v>56</v>
       </c>
       <c r="D21" s="2"/>
     </row>
@@ -1590,11 +1612,11 @@
       <c r="A22" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B22" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>32</v>
+      <c r="B22" t="s">
+        <v>27</v>
+      </c>
+      <c r="C22" t="s">
+        <v>28</v>
       </c>
       <c r="D22" s="2"/>
     </row>
@@ -1602,11 +1624,11 @@
       <c r="A23" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B23" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>39</v>
+      <c r="B23" t="s">
+        <v>162</v>
+      </c>
+      <c r="C23" t="s">
+        <v>166</v>
       </c>
       <c r="D23" s="2"/>
     </row>
@@ -1614,11 +1636,11 @@
       <c r="A24" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B24" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>43</v>
+      <c r="B24" t="s">
+        <v>31</v>
+      </c>
+      <c r="C24" t="s">
+        <v>32</v>
       </c>
       <c r="D24" s="2"/>
     </row>
@@ -1626,11 +1648,11 @@
       <c r="A25" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B25" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>139</v>
+      <c r="B25" t="s">
+        <v>38</v>
+      </c>
+      <c r="C25" t="s">
+        <v>39</v>
       </c>
       <c r="D25" s="2"/>
     </row>
@@ -1638,11 +1660,11 @@
       <c r="A26" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B26" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>141</v>
+      <c r="B26" t="s">
+        <v>42</v>
+      </c>
+      <c r="C26" t="s">
+        <v>43</v>
       </c>
       <c r="D26" s="2"/>
     </row>
@@ -1650,10 +1672,10 @@
       <c r="A27" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B27" t="s">
         <v>51</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C27" t="s">
         <v>52</v>
       </c>
       <c r="D27" s="2"/>
@@ -1662,11 +1684,11 @@
       <c r="A28" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B28" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>145</v>
+      <c r="B28" t="s">
+        <v>163</v>
+      </c>
+      <c r="C28" t="s">
+        <v>164</v>
       </c>
       <c r="D28" s="2"/>
     </row>
@@ -1674,10 +1696,10 @@
       <c r="A29" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B29" t="s">
         <v>146</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="C29" t="s">
         <v>147</v>
       </c>
       <c r="D29" s="2"/>
@@ -1686,11 +1708,11 @@
       <c r="A30" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>153</v>
+      <c r="B30" t="s">
+        <v>138</v>
+      </c>
+      <c r="C30" t="s">
+        <v>139</v>
       </c>
       <c r="D30" s="2"/>
     </row>
@@ -1698,11 +1720,11 @@
       <c r="A31" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B31" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>143</v>
+      <c r="B31" t="s">
+        <v>144</v>
+      </c>
+      <c r="C31" t="s">
+        <v>145</v>
       </c>
       <c r="D31" s="2"/>
     </row>
@@ -1710,41 +1732,47 @@
       <c r="A32" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B32" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>50</v>
+      <c r="B32" t="s">
+        <v>140</v>
+      </c>
+      <c r="C32" t="s">
+        <v>141</v>
       </c>
       <c r="D32" s="2"/>
     </row>
     <row r="33" spans="1:4">
-      <c r="A33" s="2"/>
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
+      <c r="A33" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B33" t="s">
+        <v>152</v>
+      </c>
+      <c r="C33" t="s">
+        <v>153</v>
+      </c>
       <c r="D33" s="2"/>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>102</v>
+        <v>16</v>
+      </c>
+      <c r="B34" t="s">
+        <v>142</v>
+      </c>
+      <c r="C34" t="s">
+        <v>143</v>
       </c>
       <c r="D34" s="2"/>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>103</v>
+        <v>16</v>
+      </c>
+      <c r="B35" t="s">
+        <v>49</v>
+      </c>
+      <c r="C35" t="s">
+        <v>50</v>
       </c>
       <c r="D35" s="2"/>
     </row>
@@ -1755,38 +1783,32 @@
       <c r="D36" s="2"/>
     </row>
     <row r="37" spans="1:4">
-      <c r="A37" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>80</v>
-      </c>
+      <c r="A37" s="2"/>
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
       <c r="D37" s="2"/>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="2" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>78</v>
+        <v>18</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>81</v>
+        <v>102</v>
       </c>
       <c r="D38" s="2"/>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="2" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>82</v>
+        <v>103</v>
       </c>
       <c r="D39" s="2"/>
     </row>
@@ -1798,50 +1820,44 @@
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="2" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>93</v>
+        <v>77</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="D41" s="2"/>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="2" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>156</v>
+        <v>78</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>157</v>
+        <v>81</v>
       </c>
       <c r="D42" s="2"/>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="2" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>158</v>
+        <v>82</v>
       </c>
       <c r="D43" s="2"/>
     </row>
     <row r="44" spans="1:4">
-      <c r="A44" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>160</v>
-      </c>
+      <c r="A44" s="2"/>
+      <c r="B44" s="2"/>
+      <c r="C44" s="2"/>
       <c r="D44" s="2"/>
     </row>
     <row r="45" spans="1:4">
@@ -1849,10 +1865,10 @@
         <v>90</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D45" s="2"/>
     </row>
@@ -1861,10 +1877,10 @@
         <v>90</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>95</v>
+        <v>156</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>98</v>
+        <v>157</v>
       </c>
       <c r="D46" s="2"/>
     </row>
@@ -1873,10 +1889,10 @@
         <v>90</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>99</v>
+        <v>158</v>
       </c>
       <c r="D47" s="2"/>
     </row>
@@ -1885,12 +1901,60 @@
         <v>90</v>
       </c>
       <c r="B48" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="D48" s="2"/>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D49" s="2"/>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D50" s="2"/>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="A51" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D51" s="2"/>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B52" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="C48" s="2" t="s">
+      <c r="C52" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="D48" s="2"/>
+      <c r="D52" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
add known_by to students
</commit_message>
<xml_diff>
--- a/ona_forms/asistencias-pagos.xlsx
+++ b/ona_forms/asistencias-pagos.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="32880" windowHeight="16940" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="177">
   <si>
     <t>type</t>
   </si>
@@ -515,6 +515,42 @@
   </si>
   <si>
     <t>Limbo 3 - Intermedios 2 - Jueves Vera</t>
+  </si>
+  <si>
+    <t>Nos conocio por…</t>
+  </si>
+  <si>
+    <t>known_by</t>
+  </si>
+  <si>
+    <t>select_one known_type</t>
+  </si>
+  <si>
+    <t>known_type</t>
+  </si>
+  <si>
+    <t>Facebook</t>
+  </si>
+  <si>
+    <t>Google</t>
+  </si>
+  <si>
+    <t>Amigos</t>
+  </si>
+  <si>
+    <t>Ya la conocía por la escena</t>
+  </si>
+  <si>
+    <t>facebook</t>
+  </si>
+  <si>
+    <t>google</t>
+  </si>
+  <si>
+    <t>friends</t>
+  </si>
+  <si>
+    <t>already_known</t>
   </si>
 </sst>
 </file>
@@ -586,7 +622,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="26">
+  <cellStyleXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -613,13 +649,20 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="26">
+  <cellStyles count="32">
     <cellStyle name="Bold text" xfId="4"/>
     <cellStyle name="Col header" xfId="8"/>
     <cellStyle name="Date" xfId="9"/>
@@ -632,6 +675,9 @@
     <cellStyle name="Followed Hyperlink" xfId="21" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="23" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="25" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="27" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="29" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="31" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="12" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="14" builtinId="8" hidden="1"/>
@@ -640,6 +686,9 @@
     <cellStyle name="Hyperlink" xfId="20" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="22" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="24" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="26" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="28" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="30" builtinId="8" hidden="1"/>
     <cellStyle name="Money" xfId="6"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Number" xfId="5"/>
@@ -979,10 +1028,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K22"/>
+  <dimension ref="A1:K23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1246,95 +1295,110 @@
     </row>
     <row r="16" spans="1:11">
       <c r="A16" t="s">
-        <v>65</v>
+        <v>167</v>
       </c>
       <c r="B16" t="s">
-        <v>73</v>
+        <v>166</v>
       </c>
       <c r="C16" t="s">
-        <v>119</v>
-      </c>
-      <c r="D16" t="s">
-        <v>133</v>
-      </c>
-      <c r="I16" t="s">
-        <v>67</v>
+        <v>165</v>
+      </c>
+      <c r="H16" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="17" spans="1:10">
       <c r="A17" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B17" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="C17" t="s">
-        <v>120</v>
-      </c>
-      <c r="H17" t="s">
-        <v>74</v>
+        <v>119</v>
+      </c>
+      <c r="D17" t="s">
+        <v>133</v>
+      </c>
+      <c r="I17" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="18" spans="1:10">
       <c r="A18" t="s">
-        <v>100</v>
+        <v>69</v>
       </c>
       <c r="B18" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C18" t="s">
-        <v>121</v>
-      </c>
-      <c r="D18" t="s">
-        <v>134</v>
+        <v>120</v>
+      </c>
+      <c r="H18" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="19" spans="1:10">
       <c r="A19" t="s">
-        <v>89</v>
+        <v>100</v>
       </c>
       <c r="B19" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C19" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D19" t="s">
-        <v>135</v>
-      </c>
-      <c r="H19" t="s">
-        <v>106</v>
+        <v>134</v>
       </c>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" t="s">
-        <v>70</v>
+        <v>89</v>
+      </c>
+      <c r="B20" t="s">
+        <v>71</v>
+      </c>
+      <c r="C20" t="s">
+        <v>122</v>
+      </c>
+      <c r="D20" t="s">
+        <v>135</v>
+      </c>
+      <c r="H20" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
     </row>
     <row r="22" spans="1:10">
       <c r="A22" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="A23" t="s">
         <v>61</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B23" t="s">
         <v>123</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C23" t="s">
         <v>124</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D23" t="s">
         <v>136</v>
       </c>
-      <c r="J22" t="s">
+      <c r="J23" t="s">
         <v>125</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1345,10 +1409,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D51"/>
+  <dimension ref="A1:D56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="A54" sqref="A54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1942,6 +2006,50 @@
       </c>
       <c r="D51" s="2"/>
     </row>
+    <row r="53" spans="1:4">
+      <c r="A53" t="s">
+        <v>168</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
+      <c r="A54" t="s">
+        <v>168</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
+      <c r="A55" t="s">
+        <v>168</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="A56" t="s">
+        <v>168</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>172</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
remove Sc and old place's names from courses if given in Swing City HQ. update course and packs in ona_forms
</commit_message>
<xml_diff>
--- a/ona_forms/asistencias-pagos.xlsx
+++ b/ona_forms/asistencias-pagos.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="1360" yWindow="140" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="193">
   <si>
     <t>type</t>
   </si>
@@ -106,75 +106,42 @@
     <t>CH_PRIN_MIE</t>
   </si>
   <si>
-    <t>Charleston - Principiantes - Miércoles Sendas</t>
-  </si>
-  <si>
     <t>LH_AVAN_LUN</t>
   </si>
   <si>
-    <t>Lindy Hop - Avanzados - Lunes colmegna</t>
-  </si>
-  <si>
     <t>LH_INT1_JUE</t>
   </si>
   <si>
-    <t>Lindy Hop - Intermedios 1 - Jueves Vera</t>
-  </si>
-  <si>
     <t>LH_INT1_LUN</t>
   </si>
   <si>
-    <t>Lindy Hop - Intermedios 1 - Lunes colmegna</t>
-  </si>
-  <si>
     <t>LH_INT1_MAR</t>
   </si>
   <si>
     <t>LH_INT1_MIE</t>
   </si>
   <si>
-    <t>Lindy Hop - Intermedios 1 - Miércoles Vera</t>
-  </si>
-  <si>
     <t>LH_INT2_JUE</t>
   </si>
   <si>
-    <t>Lindy Hop - Intermedios 2 - Jueves Vera</t>
-  </si>
-  <si>
     <t>LH_INT2_LUN</t>
   </si>
   <si>
-    <t>Lindy Hop - Intermedios 2 - Lunes colmegna</t>
-  </si>
-  <si>
     <t>LH_PRIN_JUE</t>
   </si>
   <si>
-    <t>Lindy Hop - Principiantes - Jueves Vera</t>
-  </si>
-  <si>
     <t>LH_PRIN_LUN</t>
   </si>
   <si>
-    <t>Lindy Hop - Principiantes - Lunes colmegna</t>
-  </si>
-  <si>
     <t>LH_PRIN_MAR2</t>
   </si>
   <si>
     <t>LH_PRIN_MIE2</t>
   </si>
   <si>
-    <t>Lindy Hop - Principiantes - Miércoles Vera</t>
-  </si>
-  <si>
     <t>LH_PRIN_SAB</t>
   </si>
   <si>
-    <t>Lindy Hop - Principiantes - Sábados Sc</t>
-  </si>
-  <si>
     <t>LH_PRIN_VIE</t>
   </si>
   <si>
@@ -184,15 +151,9 @@
     <t>TP_INT1_MAR</t>
   </si>
   <si>
-    <t>Tap - Intermedios 1 - Martes La huella</t>
-  </si>
-  <si>
     <t>CH_AVAN_MIE</t>
   </si>
   <si>
-    <t>Charleston - Avanzados - Miércoles Sendas</t>
-  </si>
-  <si>
     <t>begin repeat</t>
   </si>
   <si>
@@ -304,24 +265,12 @@
     <t>3_MESES</t>
   </si>
   <si>
-    <t>3 Meses 1 x Semana $550</t>
-  </si>
-  <si>
     <t>1_X_SEMANA_5</t>
   </si>
   <si>
     <t>1_X_SEMANA_4</t>
   </si>
   <si>
-    <t>Mensual 1 x Semana (4 c) $250</t>
-  </si>
-  <si>
-    <t>Mensual 1 x Semana (5 c) $300</t>
-  </si>
-  <si>
-    <t>Clase suelta $70</t>
-  </si>
-  <si>
     <t>select_one payment_type</t>
   </si>
   <si>
@@ -445,21 +394,12 @@
     <t>LH_INT2_SAB</t>
   </si>
   <si>
-    <t>Lindy Hop - Intermedios 2 - Sábados Sc</t>
-  </si>
-  <si>
     <t>TP_INT1_VIE</t>
   </si>
   <si>
-    <t>Tap - Intermedios 1 - Viernes La huella</t>
-  </si>
-  <si>
     <t>TP_PRIN_VIE</t>
   </si>
   <si>
-    <t>Tap - Principiantes - Viernes La huella</t>
-  </si>
-  <si>
     <t>note</t>
   </si>
   <si>
@@ -475,48 +415,21 @@
     <t>LH_INT1_SAB</t>
   </si>
   <si>
-    <t>Lindy Hop - Intermedios 1 - Sábados Sc</t>
-  </si>
-  <si>
-    <t>Lindy Hop - Intermedios 1 - Martes La Fragua</t>
-  </si>
-  <si>
-    <t>Lindy Hop - Principiantes - Martes La Fragua</t>
-  </si>
-  <si>
     <t>3_X_SEMANA</t>
   </si>
   <si>
-    <t>Mensual 3 x Semana $500</t>
-  </si>
-  <si>
-    <t>Mensual 2 x Semana $400</t>
-  </si>
-  <si>
     <t>1_X_SEMANA_3</t>
   </si>
   <si>
-    <t>Mensual 1 x Semana (3 c) $180</t>
-  </si>
-  <si>
     <t>LIMBO_2</t>
   </si>
   <si>
     <t>LIMBO_1</t>
   </si>
   <si>
-    <t>Limbo 2 - Intermedios 1 - Miércoles Sendas</t>
-  </si>
-  <si>
-    <t>Limbo 1 - Principiantes - Miércoles Sendas</t>
-  </si>
-  <si>
     <t>LIMBO_3_JUE</t>
   </si>
   <si>
-    <t>Limbo 3 - Intermedios 2 - Jueves Vera</t>
-  </si>
-  <si>
     <t>Nos conocio por…</t>
   </si>
   <si>
@@ -551,6 +464,141 @@
   </si>
   <si>
     <t>already_known</t>
+  </si>
+  <si>
+    <t>LIBRE</t>
+  </si>
+  <si>
+    <t>1 Mes. Libre $1000</t>
+  </si>
+  <si>
+    <t>3 Meses 1 x Semana $720</t>
+  </si>
+  <si>
+    <t>Mensual 3 x Semana $650</t>
+  </si>
+  <si>
+    <t>Mensual 2 x Semana $520</t>
+  </si>
+  <si>
+    <t>Mensual 1 x Semana (3 c) $230</t>
+  </si>
+  <si>
+    <t>Mensual 1 x Semana (4 c) $320</t>
+  </si>
+  <si>
+    <t>Mensual 1 x Semana (5 c) $390</t>
+  </si>
+  <si>
+    <t>Clase suelta $90</t>
+  </si>
+  <si>
+    <t>Lindy Hop - Intermedios 2 - Lunes</t>
+  </si>
+  <si>
+    <t>Lindy Hop - Principiantes - Lunes</t>
+  </si>
+  <si>
+    <t>Lindy Hop - Avanzados - Lunes</t>
+  </si>
+  <si>
+    <t>Lindy Hop - Intermedios 1 - Lunes</t>
+  </si>
+  <si>
+    <t>Tap - Intermedios 1 - Martes</t>
+  </si>
+  <si>
+    <t>LH_AVAN2_MAR</t>
+  </si>
+  <si>
+    <t>Lindy Hop - Avanzados 2 - Martes</t>
+  </si>
+  <si>
+    <t>Lindy Hop - Intermedios 1 - Martes</t>
+  </si>
+  <si>
+    <t>TP_PRIN_MAR2</t>
+  </si>
+  <si>
+    <t>Tap - Principiantes - Martes</t>
+  </si>
+  <si>
+    <t>LH_INT3_MAR</t>
+  </si>
+  <si>
+    <t>Lindy Hop - Intermedios 3 - Martes</t>
+  </si>
+  <si>
+    <t>Lindy Hop - Principiantes - Martes</t>
+  </si>
+  <si>
+    <t>Charleston - Principiantes - Miércoles</t>
+  </si>
+  <si>
+    <t>Lindy Hop - Intermedios 1 - Miércoles</t>
+  </si>
+  <si>
+    <t>Limbo 2 - Intermedios 1 - Miércoles</t>
+  </si>
+  <si>
+    <t>Charleston - Avanzados - Miércoles</t>
+  </si>
+  <si>
+    <t>Lindy Hop - Principiantes - Miércoles</t>
+  </si>
+  <si>
+    <t>Limbo 1 - Principiantes - Miércoles</t>
+  </si>
+  <si>
+    <t>Lindy Hop - Intermedios 1 - Jueves</t>
+  </si>
+  <si>
+    <t>Limbo 3 - Intermedios 2 - Jueves</t>
+  </si>
+  <si>
+    <t>Lindy Hop - Intermedios 2 - Jueves</t>
+  </si>
+  <si>
+    <t>Lindy Hop - Principiantes - Jueves</t>
+  </si>
+  <si>
+    <t>LH_PRIN_VIE2</t>
+  </si>
+  <si>
+    <t>Lindy Hop - Principiantes - Viernes</t>
+  </si>
+  <si>
+    <t>Tap - Principiantes - Viernes</t>
+  </si>
+  <si>
+    <t>LH_INT1_VIE_SC</t>
+  </si>
+  <si>
+    <t>Lindy Hop - Intermedios 1 - Viernes</t>
+  </si>
+  <si>
+    <t>Tap - Intermedios 1 - Viernes</t>
+  </si>
+  <si>
+    <t>LH_AVAN_SAB</t>
+  </si>
+  <si>
+    <t>Lindy Hop - Avanzados - Sábados</t>
+  </si>
+  <si>
+    <t>CH_AVAN_SAB</t>
+  </si>
+  <si>
+    <t>Charleston - Avanzados - Sábados</t>
+  </si>
+  <si>
+    <t>Lindy Hop - Intermedios 1 - Sábados</t>
+  </si>
+  <si>
+    <t>Lindy Hop - Intermedios 2 - Sábados</t>
+  </si>
+  <si>
+    <t>Lindy Hop - Principiantes - Sábados</t>
   </si>
 </sst>
 </file>
@@ -622,7 +670,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="32">
+  <cellStyleXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -655,6 +703,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -662,7 +712,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="32">
+  <cellStyles count="34">
     <cellStyle name="Bold text" xfId="4"/>
     <cellStyle name="Col header" xfId="8"/>
     <cellStyle name="Date" xfId="9"/>
@@ -678,6 +728,7 @@
     <cellStyle name="Followed Hyperlink" xfId="27" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="29" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="31" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="33" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="12" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="14" builtinId="8" hidden="1"/>
@@ -689,6 +740,7 @@
     <cellStyle name="Hyperlink" xfId="26" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="28" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="30" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="32" builtinId="8" hidden="1"/>
     <cellStyle name="Money" xfId="6"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Number" xfId="5"/>
@@ -1097,16 +1149,16 @@
     </row>
     <row r="4" spans="1:11">
       <c r="A4" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="B4" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="C4" t="s">
-        <v>108</v>
+        <v>91</v>
       </c>
       <c r="D4" t="s">
-        <v>126</v>
+        <v>109</v>
       </c>
       <c r="E4" t="s">
         <v>18</v>
@@ -1115,7 +1167,7 @@
         <v>13</v>
       </c>
       <c r="J4" t="s">
-        <v>101</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -1129,7 +1181,7 @@
         <v>17</v>
       </c>
       <c r="D5" t="s">
-        <v>127</v>
+        <v>110</v>
       </c>
       <c r="E5" t="s">
         <v>18</v>
@@ -1137,16 +1189,16 @@
     </row>
     <row r="6" spans="1:11">
       <c r="A6" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="B6" t="s">
         <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>109</v>
+        <v>92</v>
       </c>
       <c r="D6" t="s">
-        <v>128</v>
+        <v>111</v>
       </c>
       <c r="E6" t="s">
         <v>18</v>
@@ -1154,251 +1206,250 @@
     </row>
     <row r="7" spans="1:11">
       <c r="A7" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="B7" t="s">
-        <v>107</v>
+        <v>90</v>
       </c>
       <c r="C7" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="D7" t="s">
-        <v>129</v>
+        <v>112</v>
       </c>
     </row>
     <row r="8" spans="1:11">
       <c r="A8" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="B8" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="C8" t="s">
-        <v>111</v>
+        <v>94</v>
       </c>
     </row>
     <row r="9" spans="1:11">
       <c r="A9" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="B9" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="C9" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="E9" t="s">
         <v>18</v>
       </c>
       <c r="I9" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:11">
       <c r="A10" t="s">
-        <v>146</v>
+        <v>126</v>
       </c>
       <c r="B10" t="s">
-        <v>147</v>
+        <v>127</v>
       </c>
       <c r="D10" t="s">
-        <v>148</v>
+        <v>128</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>149</v>
+        <v>129</v>
       </c>
     </row>
     <row r="11" spans="1:11">
       <c r="A11" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="B11" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="C11" t="s">
-        <v>112</v>
+        <v>95</v>
       </c>
       <c r="D11" t="s">
-        <v>130</v>
+        <v>113</v>
       </c>
       <c r="H11" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
     </row>
     <row r="12" spans="1:11">
       <c r="A12" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="B12" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="C12" t="s">
-        <v>113</v>
+        <v>96</v>
       </c>
       <c r="D12" t="s">
-        <v>131</v>
+        <v>114</v>
       </c>
       <c r="H12" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
     </row>
     <row r="13" spans="1:11">
       <c r="A13" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="B13" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="C13" t="s">
-        <v>114</v>
+        <v>97</v>
       </c>
       <c r="D13" t="s">
-        <v>132</v>
+        <v>115</v>
       </c>
       <c r="E13" t="s">
         <v>18</v>
       </c>
       <c r="H13" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
     </row>
     <row r="14" spans="1:11">
       <c r="A14" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="B14" t="s">
-        <v>116</v>
+        <v>99</v>
       </c>
       <c r="C14" t="s">
-        <v>115</v>
+        <v>98</v>
       </c>
       <c r="E14" t="s">
         <v>18</v>
       </c>
       <c r="H14" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
     </row>
     <row r="15" spans="1:11">
       <c r="A15" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="B15" t="s">
-        <v>117</v>
+        <v>100</v>
       </c>
       <c r="C15" t="s">
-        <v>118</v>
+        <v>101</v>
       </c>
       <c r="H15" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
     </row>
     <row r="16" spans="1:11">
       <c r="A16" t="s">
-        <v>167</v>
+        <v>138</v>
       </c>
       <c r="B16" t="s">
-        <v>166</v>
+        <v>137</v>
       </c>
       <c r="C16" t="s">
-        <v>165</v>
+        <v>136</v>
       </c>
       <c r="H16" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
     </row>
     <row r="17" spans="1:10">
       <c r="A17" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="B17" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="C17" t="s">
-        <v>119</v>
+        <v>102</v>
       </c>
       <c r="D17" t="s">
-        <v>133</v>
+        <v>116</v>
       </c>
       <c r="I17" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
     </row>
     <row r="18" spans="1:10">
       <c r="A18" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="B18" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="C18" t="s">
-        <v>120</v>
+        <v>103</v>
       </c>
       <c r="H18" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
     </row>
     <row r="19" spans="1:10">
       <c r="A19" t="s">
-        <v>100</v>
+        <v>83</v>
       </c>
       <c r="B19" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="C19" t="s">
-        <v>121</v>
+        <v>104</v>
       </c>
       <c r="D19" t="s">
-        <v>134</v>
+        <v>117</v>
       </c>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" t="s">
+        <v>76</v>
+      </c>
+      <c r="B20" t="s">
+        <v>58</v>
+      </c>
+      <c r="C20" t="s">
+        <v>105</v>
+      </c>
+      <c r="D20" t="s">
+        <v>118</v>
+      </c>
+      <c r="H20" t="s">
         <v>89</v>
-      </c>
-      <c r="B20" t="s">
-        <v>71</v>
-      </c>
-      <c r="C20" t="s">
-        <v>122</v>
-      </c>
-      <c r="D20" t="s">
-        <v>135</v>
-      </c>
-      <c r="H20" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
     </row>
     <row r="22" spans="1:10">
       <c r="A22" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
     </row>
     <row r="23" spans="1:10">
       <c r="A23" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="B23" t="s">
-        <v>123</v>
+        <v>106</v>
       </c>
       <c r="C23" t="s">
-        <v>124</v>
+        <v>107</v>
       </c>
       <c r="D23" t="s">
-        <v>136</v>
+        <v>119</v>
       </c>
       <c r="J23" t="s">
-        <v>125</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1409,10 +1460,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D56"/>
+  <dimension ref="A1:D63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A54" sqref="A54"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1525,10 +1576,10 @@
         <v>15</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>137</v>
+        <v>120</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>137</v>
+        <v>120</v>
       </c>
       <c r="D9" s="2"/>
     </row>
@@ -1542,10 +1593,10 @@
       <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="2" t="s">
         <v>41</v>
       </c>
       <c r="D11" s="2"/>
@@ -1554,11 +1605,11 @@
       <c r="A12" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B12" t="s">
-        <v>44</v>
-      </c>
-      <c r="C12" t="s">
-        <v>45</v>
+      <c r="B12" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>122</v>
       </c>
       <c r="D12" s="2"/>
     </row>
@@ -1566,11 +1617,11 @@
       <c r="A13" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B13" t="s">
-        <v>29</v>
-      </c>
-      <c r="C13" t="s">
-        <v>30</v>
+      <c r="B13" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>157</v>
       </c>
       <c r="D13" s="2"/>
     </row>
@@ -1578,11 +1629,11 @@
       <c r="A14" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B14" t="s">
-        <v>33</v>
-      </c>
-      <c r="C14" t="s">
-        <v>34</v>
+      <c r="B14" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>158</v>
       </c>
       <c r="D14" s="2"/>
     </row>
@@ -1590,11 +1641,11 @@
       <c r="A15" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B15" t="s">
-        <v>53</v>
-      </c>
-      <c r="C15" t="s">
-        <v>54</v>
+      <c r="B15" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>159</v>
       </c>
       <c r="D15" s="2"/>
     </row>
@@ -1602,11 +1653,11 @@
       <c r="A16" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B16" t="s">
-        <v>35</v>
-      </c>
-      <c r="C16" t="s">
-        <v>152</v>
+      <c r="B16" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>160</v>
       </c>
       <c r="D16" s="2"/>
     </row>
@@ -1614,11 +1665,11 @@
       <c r="A17" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B17" t="s">
-        <v>46</v>
-      </c>
-      <c r="C17" t="s">
-        <v>153</v>
+      <c r="B17" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>161</v>
       </c>
       <c r="D17" s="2"/>
     </row>
@@ -1626,11 +1677,11 @@
       <c r="A18" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B18" t="s">
-        <v>36</v>
-      </c>
-      <c r="C18" t="s">
-        <v>37</v>
+      <c r="B18" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>163</v>
       </c>
       <c r="D18" s="2"/>
     </row>
@@ -1638,11 +1689,11 @@
       <c r="A19" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B19" t="s">
-        <v>47</v>
-      </c>
-      <c r="C19" t="s">
-        <v>48</v>
+      <c r="B19" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>164</v>
       </c>
       <c r="D19" s="2"/>
     </row>
@@ -1650,11 +1701,11 @@
       <c r="A20" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B20" t="s">
-        <v>159</v>
-      </c>
-      <c r="C20" t="s">
-        <v>161</v>
+      <c r="B20" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>166</v>
       </c>
       <c r="D20" s="2"/>
     </row>
@@ -1662,11 +1713,11 @@
       <c r="A21" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B21" t="s">
-        <v>55</v>
-      </c>
-      <c r="C21" t="s">
-        <v>56</v>
+      <c r="B21" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>168</v>
       </c>
       <c r="D21" s="2"/>
     </row>
@@ -1674,11 +1725,11 @@
       <c r="A22" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B22" t="s">
-        <v>27</v>
-      </c>
-      <c r="C22" t="s">
-        <v>28</v>
+      <c r="B22" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>169</v>
       </c>
       <c r="D22" s="2"/>
     </row>
@@ -1686,11 +1737,11 @@
       <c r="A23" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B23" t="s">
-        <v>160</v>
-      </c>
-      <c r="C23" t="s">
-        <v>162</v>
+      <c r="B23" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>170</v>
       </c>
       <c r="D23" s="2"/>
     </row>
@@ -1698,11 +1749,11 @@
       <c r="A24" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B24" t="s">
-        <v>31</v>
-      </c>
-      <c r="C24" t="s">
+      <c r="B24" s="2" t="s">
         <v>32</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>171</v>
       </c>
       <c r="D24" s="2"/>
     </row>
@@ -1710,11 +1761,11 @@
       <c r="A25" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B25" t="s">
-        <v>38</v>
-      </c>
-      <c r="C25" t="s">
-        <v>39</v>
+      <c r="B25" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>172</v>
       </c>
       <c r="D25" s="2"/>
     </row>
@@ -1722,11 +1773,11 @@
       <c r="A26" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B26" t="s">
-        <v>42</v>
-      </c>
-      <c r="C26" t="s">
+      <c r="B26" s="2" t="s">
         <v>43</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>173</v>
       </c>
       <c r="D26" s="2"/>
     </row>
@@ -1734,11 +1785,11 @@
       <c r="A27" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B27" t="s">
-        <v>163</v>
-      </c>
-      <c r="C27" t="s">
-        <v>164</v>
+      <c r="B27" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>174</v>
       </c>
       <c r="D27" s="2"/>
     </row>
@@ -1746,11 +1797,11 @@
       <c r="A28" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B28" t="s">
-        <v>51</v>
-      </c>
-      <c r="C28" t="s">
-        <v>52</v>
+      <c r="B28" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>175</v>
       </c>
       <c r="D28" s="2"/>
     </row>
@@ -1758,11 +1809,11 @@
       <c r="A29" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B29" t="s">
-        <v>144</v>
-      </c>
-      <c r="C29" t="s">
-        <v>145</v>
+      <c r="B29" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>176</v>
       </c>
       <c r="D29" s="2"/>
     </row>
@@ -1770,11 +1821,11 @@
       <c r="A30" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B30" t="s">
-        <v>138</v>
-      </c>
-      <c r="C30" t="s">
-        <v>139</v>
+      <c r="B30" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>177</v>
       </c>
       <c r="D30" s="2"/>
     </row>
@@ -1782,11 +1833,11 @@
       <c r="A31" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B31" t="s">
-        <v>142</v>
-      </c>
-      <c r="C31" t="s">
-        <v>143</v>
+      <c r="B31" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>178</v>
       </c>
       <c r="D31" s="2"/>
     </row>
@@ -1794,11 +1845,11 @@
       <c r="A32" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B32" t="s">
-        <v>150</v>
-      </c>
-      <c r="C32" t="s">
-        <v>151</v>
+      <c r="B32" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>179</v>
       </c>
       <c r="D32" s="2"/>
     </row>
@@ -1806,11 +1857,11 @@
       <c r="A33" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B33" t="s">
-        <v>140</v>
-      </c>
-      <c r="C33" t="s">
-        <v>141</v>
+      <c r="B33" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>181</v>
       </c>
       <c r="D33" s="2"/>
     </row>
@@ -1818,236 +1869,326 @@
       <c r="A34" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B34" t="s">
-        <v>49</v>
-      </c>
-      <c r="C34" t="s">
-        <v>50</v>
+      <c r="B34" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>182</v>
       </c>
       <c r="D34" s="2"/>
     </row>
     <row r="35" spans="1:4">
-      <c r="A35" s="2"/>
-      <c r="B35" s="2"/>
-      <c r="C35" s="2"/>
+      <c r="A35" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>184</v>
+      </c>
       <c r="D35" s="2"/>
     </row>
     <row r="36" spans="1:4">
-      <c r="A36" s="2"/>
-      <c r="B36" s="2"/>
-      <c r="C36" s="2"/>
+      <c r="A36" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>185</v>
+      </c>
       <c r="D36" s="2"/>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="2" t="s">
-        <v>66</v>
+        <v>16</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>18</v>
+        <v>186</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>102</v>
+        <v>187</v>
       </c>
       <c r="D37" s="2"/>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="2" t="s">
-        <v>66</v>
+        <v>16</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>67</v>
+        <v>188</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>103</v>
+        <v>189</v>
       </c>
       <c r="D38" s="2"/>
     </row>
     <row r="39" spans="1:4">
-      <c r="A39" s="2"/>
-      <c r="B39" s="2"/>
-      <c r="C39" s="2"/>
+      <c r="A39" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>190</v>
+      </c>
       <c r="D39" s="2"/>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="2" t="s">
-        <v>76</v>
+        <v>16</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>77</v>
+        <v>123</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>80</v>
+        <v>191</v>
       </c>
       <c r="D40" s="2"/>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="2" t="s">
-        <v>76</v>
+        <v>16</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>78</v>
+        <v>39</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>81</v>
+        <v>192</v>
       </c>
       <c r="D41" s="2"/>
     </row>
     <row r="42" spans="1:4">
-      <c r="A42" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>82</v>
-      </c>
+      <c r="A42" s="2"/>
+      <c r="B42" s="2"/>
+      <c r="C42" s="2"/>
       <c r="D42" s="2"/>
     </row>
     <row r="43" spans="1:4">
-      <c r="A43" s="2"/>
-      <c r="B43" s="2"/>
-      <c r="C43" s="2"/>
+      <c r="A43" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>85</v>
+      </c>
       <c r="D43" s="2"/>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="2" t="s">
-        <v>90</v>
+        <v>53</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>93</v>
+        <v>54</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="D44" s="2"/>
     </row>
     <row r="45" spans="1:4">
-      <c r="A45" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>155</v>
-      </c>
+      <c r="A45" s="2"/>
+      <c r="B45" s="2"/>
+      <c r="C45" s="2"/>
       <c r="D45" s="2"/>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="2" t="s">
-        <v>90</v>
+        <v>63</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>91</v>
+        <v>64</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>156</v>
+        <v>67</v>
       </c>
       <c r="D46" s="2"/>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="2" t="s">
-        <v>90</v>
+        <v>63</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>157</v>
+        <v>65</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>158</v>
+        <v>68</v>
       </c>
       <c r="D47" s="2"/>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="2" t="s">
-        <v>90</v>
+        <v>63</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>96</v>
+        <v>66</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>97</v>
+        <v>69</v>
       </c>
       <c r="D48" s="2"/>
     </row>
     <row r="49" spans="1:4">
-      <c r="A49" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>98</v>
-      </c>
+      <c r="A49" s="2"/>
+      <c r="B49" s="2"/>
+      <c r="C49" s="2"/>
       <c r="D49" s="2"/>
     </row>
     <row r="50" spans="1:4">
       <c r="A50" s="2" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>92</v>
+        <v>148</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>99</v>
+        <v>149</v>
       </c>
       <c r="D50" s="2"/>
     </row>
     <row r="51" spans="1:4">
       <c r="A51" s="2" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>104</v>
+        <v>80</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>105</v>
+        <v>150</v>
       </c>
       <c r="D51" s="2"/>
     </row>
+    <row r="52" spans="1:4">
+      <c r="A52" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="D52" s="2"/>
+    </row>
     <row r="53" spans="1:4">
-      <c r="A53" t="s">
-        <v>168</v>
-      </c>
-      <c r="B53" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="C53" s="3" t="s">
-        <v>169</v>
-      </c>
+      <c r="A53" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="D53" s="2"/>
     </row>
     <row r="54" spans="1:4">
-      <c r="A54" t="s">
-        <v>168</v>
-      </c>
-      <c r="B54" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="C54" s="3" t="s">
-        <v>170</v>
-      </c>
+      <c r="A54" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="D54" s="2"/>
     </row>
     <row r="55" spans="1:4">
-      <c r="A55" t="s">
-        <v>168</v>
-      </c>
-      <c r="B55" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="C55" s="3" t="s">
-        <v>171</v>
-      </c>
+      <c r="A55" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="D55" s="2"/>
     </row>
     <row r="56" spans="1:4">
-      <c r="A56" t="s">
-        <v>168</v>
-      </c>
-      <c r="B56" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="C56" s="3" t="s">
-        <v>172</v>
+      <c r="A56" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="D56" s="2"/>
+    </row>
+    <row r="57" spans="1:4">
+      <c r="A57" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="D57" s="2"/>
+    </row>
+    <row r="58" spans="1:4">
+      <c r="A58" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D58" s="2"/>
+    </row>
+    <row r="60" spans="1:4">
+      <c r="A60" t="s">
+        <v>139</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4">
+      <c r="A61" t="s">
+        <v>139</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4">
+      <c r="A62" t="s">
+        <v>139</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4">
+      <c r="A63" t="s">
+        <v>139</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>143</v>
       </c>
     </row>
   </sheetData>

</xml_diff>